<commit_message>
reference for avg_file + get data from gen_file
</commit_message>
<xml_diff>
--- a/ПримерОбъединения.xlsx
+++ b/ПримерОбъединения.xlsx
@@ -451,7 +451,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
@@ -460,7 +460,7 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="10" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
+    <col width="90" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -1475,7 +1475,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
@@ -1484,7 +1484,7 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="10" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
+    <col width="90" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -2788,7 +2788,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="20" customWidth="1" min="4" max="4"/>
     <col width="15" customWidth="1" min="5" max="5"/>
@@ -2797,7 +2797,7 @@
     <col width="15" customWidth="1" min="8" max="8"/>
     <col width="10" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
+    <col width="90" customWidth="1" min="11" max="11"/>
     <col width="20" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
@@ -3936,17 +3936,18 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="10" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
     <col width="10" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="60" customWidth="1" min="11" max="11"/>
+    <col width="10" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="20" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -3955,7 +3956,6 @@
           <t>ЖД тариф  из портов Дальнего Востока+ Drop off</t>
         </is>
       </c>
-      <c r="M1" s="6" t="n"/>
       <c r="N1" s="6" t="n"/>
     </row>
     <row r="2">
@@ -3964,7 +3964,9 @@
       <c r="C2" s="6" t="n"/>
       <c r="D2" s="6" t="n"/>
       <c r="E2" s="6" t="n"/>
+      <c r="F2" s="6" t="n"/>
       <c r="G2" s="6" t="n"/>
+      <c r="H2" s="6" t="n"/>
       <c r="I2" s="6" t="inlineStr">
         <is>
           <t>валидность  ставки</t>
@@ -3976,7 +3978,6 @@
           <t>Drop-off Москва</t>
         </is>
       </c>
-      <c r="M2" s="6" t="n"/>
       <c r="N2" s="6" t="n"/>
     </row>
     <row r="3">
@@ -4424,11 +4425,10 @@
       <c r="N13" s="6" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:M1"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L2:M2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4448,18 +4448,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="20" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="35" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
     <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
     <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="100" customWidth="1" min="11" max="11"/>
-    <col width="20" customWidth="1" min="12" max="12"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
+    <col width="80" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4479,8 +4479,12 @@
           <t xml:space="preserve">20' </t>
         </is>
       </c>
-      <c r="G2" s="6" t="n"/>
-      <c r="I2" s="6" t="n"/>
+      <c r="H2" s="6" t="inlineStr">
+        <is>
+          <t>40'</t>
+        </is>
+      </c>
+      <c r="J2" s="6" t="n"/>
       <c r="K2" s="6" t="n"/>
       <c r="L2" s="6" t="n"/>
     </row>
@@ -9943,11 +9947,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="A1:L1"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>